<commit_message>
Corregido arbol de elementos (excel e informe)
</commit_message>
<xml_diff>
--- a/2- Emparrillado/Emparrillado.xlsx
+++ b/2- Emparrillado/Emparrillado.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935"/>
@@ -10,7 +10,7 @@
     <sheet name="Emparrillado" sheetId="1" r:id="rId1"/>
     <sheet name="Distancias entre Elementos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -89,9 +89,6 @@
     <t>Posición pies:</t>
   </si>
   <si>
-    <t>Soltado de la pelota:</t>
-  </si>
-  <si>
     <t>Recta</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>(E3-E6)-E4</t>
+  </si>
+  <si>
+    <t>Lugar de soltado de la pelota:</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1098,7 +1098,7 @@
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>14</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="48" t="s">
         <v>16</v>
@@ -1282,12 +1282,12 @@
         <v>16</v>
       </c>
       <c r="K7" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>17</v>
@@ -1314,12 +1314,12 @@
         <v>17</v>
       </c>
       <c r="K8" s="51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1">
       <c r="B9" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="50" t="s">
         <v>12</v>
@@ -1346,7 +1346,7 @@
         <v>12</v>
       </c>
       <c r="K9" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:11">
@@ -1354,7 +1354,7 @@
     </row>
     <row r="11" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="18" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B18" s="7" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C18" s="2"/>
       <c r="E18" s="8">
@@ -1477,14 +1477,14 @@
     </row>
     <row r="22" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B22" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2"/>
       <c r="E22" s="8">
         <v>1</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="7"/>
@@ -1508,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="7"/>
@@ -1521,14 +1521,14 @@
     </row>
     <row r="26" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2"/>
       <c r="E26" s="8">
         <v>1</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="7"/>
@@ -1540,7 +1540,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="7"/>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="7"/>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="7"/>
@@ -1577,14 +1577,14 @@
     </row>
     <row r="31" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B31" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2"/>
       <c r="E31" s="8">
         <v>1</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="7"/>
@@ -1596,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="7"/>
@@ -1606,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1619,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1640,16 +1640,16 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="55"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <f>ABS(Emparrillado!D4-Emparrillado!E4)+ABS(Emparrillado!D5-Emparrillado!E5)+ABS(Emparrillado!D6-Emparrillado!E6)+ABS(Emparrillado!D7-Emparrillado!E7)+ABS(Emparrillado!D8-Emparrillado!E8)+ABS(Emparrillado!D9-Emparrillado!E9)</f>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <f>ABS(Emparrillado!D4-Emparrillado!F4)+ABS(Emparrillado!D5-Emparrillado!F5)+ABS(Emparrillado!D6-Emparrillado!F6)+ABS(Emparrillado!D7-Emparrillado!F7)+ABS(Emparrillado!D8-Emparrillado!F8)+ ABS(Emparrillado!D9-Emparrillado!F9)</f>
@@ -1666,44 +1666,44 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="G4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="H4" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="I4" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="J4" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>57</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="O4" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="O4" s="22" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <f>ABS(Emparrillado!D4-Emparrillado!G4)+ABS(Emparrillado!D5-Emparrillado!G5)+ABS(Emparrillado!D6-Emparrillado!G6)+ABS(Emparrillado!D7-Emparrillado!G7)+ABS(Emparrillado!D8-Emparrillado!G8)+ABS(Emparrillado!D9-Emparrillado!G9)</f>
         <v>4</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="18">
@@ -1727,29 +1727,29 @@
         <v>7</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N5" s="9">
         <v>7</v>
       </c>
       <c r="O5" s="9">
         <f>MIN(M5:N5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <f>ABS(Emparrillado!D4-Emparrillado!H4)+ABS(Emparrillado!D5-Emparrillado!H5)+ABS(Emparrillado!D6-Emparrillado!H6)+ABS(Emparrillado!D7-Emparrillado!H7)+ABS(Emparrillado!D8-Emparrillado!H8)+ABS(Emparrillado!D9-Emparrillado!H9)</f>
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="10"/>
@@ -1770,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M6" s="9">
         <v>6</v>
@@ -1785,14 +1785,14 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <f>ABS(Emparrillado!D4-Emparrillado!I4)+ABS(Emparrillado!D5-Emparrillado!I5)+ABS(Emparrillado!D6-Emparrillado!I6)+ABS(Emparrillado!D7-Emparrillado!I7)+ABS(Emparrillado!D8-Emparrillado!I8)+ABS(Emparrillado!D9-Emparrillado!I9)</f>
         <v>7</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="9"/>
@@ -1810,7 +1810,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="9">
         <v>3</v>
@@ -1825,14 +1825,14 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <f>ABS(Emparrillado!E4-Emparrillado!F4)+ABS(Emparrillado!E5-Emparrillado!F5)+ABS(Emparrillado!E6-Emparrillado!F6)+ABS(Emparrillado!E7-Emparrillado!F7)+ABS(Emparrillado!E8-Emparrillado!F8)+ ABS(Emparrillado!E9-Emparrillado!F9)</f>
         <v>6</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
@@ -1847,7 +1847,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M8" s="9">
         <v>5</v>
@@ -1862,14 +1862,14 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <f>ABS(Emparrillado!E4-Emparrillado!G4)+ABS(Emparrillado!E5-Emparrillado!G5)+ABS(Emparrillado!E6-Emparrillado!G6)+ABS(Emparrillado!E7-Emparrillado!G7)+ABS(Emparrillado!E8-Emparrillado!G8)+ABS(Emparrillado!E9-Emparrillado!G9)</f>
         <v>5</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="9"/>
@@ -1883,14 +1883,14 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <f>ABS(Emparrillado!E4-Emparrillado!H4)+ABS(Emparrillado!E5-Emparrillado!H5)+ABS(Emparrillado!E6-Emparrillado!H6)+ABS(Emparrillado!E7-Emparrillado!H7)+ABS(Emparrillado!E8-Emparrillado!H8)+ABS(Emparrillado!E9-Emparrillado!H9)</f>
         <v>5</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="11"/>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <f>ABS(Emparrillado!E4-Emparrillado!I4)+ABS(Emparrillado!E5-Emparrillado!I5)+ABS(Emparrillado!E6-Emparrillado!I6)+ABS(Emparrillado!E7-Emparrillado!I7)+ABS(Emparrillado!E8-Emparrillado!I8)+ABS(Emparrillado!E9-Emparrillado!I9)</f>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <f>ABS(Emparrillado!F4-Emparrillado!G4)+ABS(Emparrillado!F5-Emparrillado!G5)+ABS(Emparrillado!F6-Emparrillado!G6)+ABS(Emparrillado!F7-Emparrillado!G7)+ABS(Emparrillado!F8-Emparrillado!G8)+ABS(Emparrillado!F9-Emparrillado!G9)</f>
@@ -1918,46 +1918,46 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="22" t="s">
-        <v>53</v>
-      </c>
       <c r="H12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="N12" s="22" t="s">
-        <v>67</v>
-      </c>
       <c r="O12" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <f>ABS(Emparrillado!F4-Emparrillado!H4)+ABS(Emparrillado!F5-Emparrillado!H5)+ABS(Emparrillado!F6-Emparrillado!H6)+ABS(Emparrillado!F7-Emparrillado!H7)+ABS(Emparrillado!F8-Emparrillado!H8)+ABS(Emparrillado!F9-Emparrillado!H9)</f>
         <v>5</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="20">
         <f>O5</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="20">
         <f>O6</f>
@@ -1972,29 +1972,29 @@
         <v>5</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N13" s="9">
         <v>6</v>
       </c>
       <c r="O13" s="9">
         <f>MIN(M13:N13)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <f>ABS(Emparrillado!F4-Emparrillado!I4)+ABS(Emparrillado!F5-Emparrillado!I5)+ABS(Emparrillado!F6-Emparrillado!I6)+ABS(Emparrillado!F7-Emparrillado!I7)+ABS(Emparrillado!F8-Emparrillado!I8)+ABS(Emparrillado!F9-Emparrillado!I9)</f>
         <v>2</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
@@ -2008,7 +2008,7 @@
         <v>4</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M14" s="9">
         <v>4</v>
@@ -2023,14 +2023,14 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <f>ABS(Emparrillado!G4-Emparrillado!H4)+ABS(Emparrillado!G5-Emparrillado!H5)+ABS(Emparrillado!G6-Emparrillado!H6)+ABS(Emparrillado!G7-Emparrillado!H7)+ABS(Emparrillado!G8-Emparrillado!H8)+ABS(Emparrillado!G9-Emparrillado!H9)</f>
         <v>4</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2042,7 +2042,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M15" s="9">
         <v>4</v>
@@ -2057,14 +2057,14 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <f>ABS(Emparrillado!G4-Emparrillado!I4)+ABS(Emparrillado!G5-Emparrillado!I5)+ABS(Emparrillado!G6-Emparrillado!I6)+ABS(Emparrillado!G7-Emparrillado!I7)+ABS(Emparrillado!G8-Emparrillado!I8)+ABS(Emparrillado!G9-Emparrillado!I9)</f>
         <v>5</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -2076,14 +2076,14 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <f>ABS(Emparrillado!H4-Emparrillado!I4)+ABS(Emparrillado!H5-Emparrillado!I5)+ABS(Emparrillado!H6-Emparrillado!I6)+ABS(Emparrillado!H7-Emparrillado!I7)+ABS(Emparrillado!H8-Emparrillado!I8)+ABS(Emparrillado!H9-Emparrillado!I9)</f>
         <v>7</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -2094,36 +2094,36 @@
     <row r="19" spans="1:15">
       <c r="D19" s="9"/>
       <c r="E19" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="N19" s="22" t="s">
-        <v>64</v>
-      </c>
       <c r="O19" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="D20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="20">
         <f>O13</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G20" s="20">
         <f>O14</f>
@@ -2134,10 +2134,10 @@
         <v>4</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M20" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N20" s="9">
         <v>4</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="D21" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
@@ -2160,7 +2160,7 @@
         <v>5</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M21" s="9">
         <v>5</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="D22" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="D23" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
@@ -2196,28 +2196,28 @@
     <row r="25" spans="1:15">
       <c r="D25" s="9"/>
       <c r="E25" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O25" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="D26" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="20">
@@ -2229,7 +2229,7 @@
         <v>4</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M26" s="9">
         <v>4</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="D27" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="28" spans="1:15">
       <c r="D28" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -2263,15 +2263,15 @@
     <row r="30" spans="1:15">
       <c r="D30" s="9"/>
       <c r="E30" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="D31" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="27">
@@ -2280,7 +2280,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="D32" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>

</xml_diff>